<commit_message>
Mise en place de la vérification des form du back-end et ajout a un depot git
</commit_message>
<xml_diff>
--- a/bdd.xlsx
+++ b/bdd.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807179BA-FC3F-4995-9E35-6C5E8C1A9886}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9B0B5E-9E9E-4FF3-AEEB-21F984DCA6F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="1845" windowWidth="34635" windowHeight="19290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bdd" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="560">
   <si>
     <t>blog_content</t>
   </si>
@@ -1981,6 +1981,18 @@
   <si>
     <t>(2, 'Autoloader nos class (static method)', '&lt;p&gt;La fonction __autoload permet de ne plus &amp;eacute;crire require pour chaque fichier de class.&lt;/p&gt;\r\n\r\n&lt;pre&gt;\r\n&lt;code class=\"language-php\"&gt;function __autoload ($class_name) {\r\n     require \'path/\'.$class_name.\'.php\';\r\n}&lt;/code&gt;&lt;/pre&gt;\r\n\r\n&lt;p&gt;Pour &amp;eacute;viter de surcharger notre code et permettre d&amp;#39;avoir une class qui peut&amp;nbsp;&amp;ecirc;tre utilis&amp;eacute; dans tous les projets nous pouvons cr&amp;eacute;er une class comme ceci&amp;nbsp;:&amp;nbsp;&lt;/p&gt;\r\n\r\n&lt;pre&gt;\r\n&lt;code class=\"language-php\"&gt;/*\r\n* class AutoLoader\r\n* Allow the autload class system\r\n*/\r\n\r\nclass Autoloader{\r\n\r\n   /**\r\n   * Save the autoloader\r\n   */\r\n   static function register(){\r\n       spl_autoload_register(array(__CLASS__, \'autoload\'));\r\n   }\r\n\r\n   /**\r\n   * Include the file corresponding to the class\r\n   * @param $class string class name\r\n   */\r\n   static function autoload($class){\r\n       require \'path/\' . $class . \'.php\';\r\n     }\r\n\r\n}&lt;/code&gt;&lt;/pre&gt;\r\n\r\n&lt;p&gt;Pour l&amp;#39;utiliser comme ceci :&lt;/p&gt;\r\n\r\n&lt;pre&gt;\r\n&lt;code class=\"language-php\"&gt;require \'path/AutoLoader.php\';\r\nAutoloader::register();&lt;/code&gt;&lt;/pre&gt;\r\n\r\n&lt;p&gt;Tout les class appel&amp;eacute;es seront automatiquement charg&amp;eacute;es.&lt;/p&gt;\r\n', NOW(), 1, 'Hadock');</t>
   </si>
+  <si>
+    <t>lenght</t>
+  </si>
+  <si>
+    <t>lenght &amp; unique</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contain a-z . A-z[3] </t>
+  </si>
 </sst>
 </file>
 
@@ -2035,7 +2047,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2058,17 +2070,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2352,15 +2410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AG22"/>
+  <dimension ref="A2:AI22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I2" s="2" t="s">
         <v>30</v>
       </c>
@@ -2388,8 +2446,10 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
     </row>
-    <row r="3" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2415,8 +2475,10 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
     </row>
-    <row r="4" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -2442,26 +2504,28 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
     </row>
-    <row r="7" spans="9:33" x14ac:dyDescent="0.25">
-      <c r="I7" s="2" t="s">
+    <row r="7" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="W7" s="2" t="s">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="5"/>
+      <c r="X7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
@@ -2471,8 +2535,10 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
     </row>
-    <row r="8" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
         <v>1</v>
       </c>
@@ -2485,20 +2551,20 @@
       <c r="M8" t="s">
         <v>12</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>1</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>2</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>3</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
         <v>9</v>
       </c>
@@ -2511,26 +2577,29 @@
       <c r="M9" t="s">
         <v>12</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>19</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>27</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>5</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>255</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>26</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
+        <v>558</v>
+      </c>
+      <c r="AD9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
         <v>15</v>
       </c>
@@ -2540,26 +2609,29 @@
       <c r="M10" t="s">
         <v>12</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>21</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>22</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>5</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>255</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>23</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
+        <v>559</v>
+      </c>
+      <c r="AD10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
         <v>13</v>
       </c>
@@ -2569,11 +2641,11 @@
       <c r="M11" t="s">
         <v>12</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
         <v>4</v>
       </c>
@@ -2587,10 +2659,13 @@
         <v>12</v>
       </c>
       <c r="N12" t="s">
+        <v>557</v>
+      </c>
+      <c r="O12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
         <v>6</v>
       </c>
@@ -2600,11 +2675,11 @@
       <c r="M13" t="s">
         <v>12</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="9:35" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
         <v>8</v>
       </c>
@@ -2618,6 +2693,9 @@
         <v>12</v>
       </c>
       <c r="N14" t="s">
+        <v>556</v>
+      </c>
+      <c r="O14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2638,9 +2716,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="I7:T7"/>
-    <mergeCell ref="W7:AG7"/>
-    <mergeCell ref="I2:AG4"/>
+    <mergeCell ref="X7:AI7"/>
+    <mergeCell ref="I2:AI4"/>
+    <mergeCell ref="I7:U7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>